<commit_message>
BRS-892-2 repairs to migration 2022/11/02
</commit_message>
<xml_diff>
--- a/migrations-data/20221102211341_data.xlsx
+++ b/migrations-data/20221102211341_data.xlsx
@@ -85,7 +85,7 @@
     <t xml:space="preserve">Wallace Island Marine Park</t>
   </si>
   <si>
-    <t xml:space="preserve">Wallace Island Marine Park - Conover Cover</t>
+    <t xml:space="preserve">Wallace Island Marine Park - Conover Cove</t>
   </si>
   <si>
     <t xml:space="preserve">No</t>
@@ -94,19 +94,19 @@
     <t xml:space="preserve">Yes</t>
   </si>
   <si>
+    <t xml:space="preserve">0473</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9954</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bodega Ridge Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bodega Ridge Park - Lover’s Leap</t>
+  </si>
+  <si>
     <t xml:space="preserve">0523</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9954</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bodega Ridge Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bodega Ridge Park - Lover’s Leap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0524</t>
   </si>
 </sst>
 </file>
@@ -238,10 +238,10 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="O8" activeCellId="0" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="43.78"/>
   </cols>
@@ -293,8 +293,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -309,31 +309,31 @@
       <c r="E2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="0" t="s">
+      <c r="H2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="0" t="s">
+      <c r="J2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="O2" s="3" t="s">

</xml_diff>

<commit_message>
transcription error with Bodega Ridge orcs
</commit_message>
<xml_diff>
--- a/migrations-data/20221102211341_data.xlsx
+++ b/migrations-data/20221102211341_data.xlsx
@@ -97,7 +97,7 @@
     <t xml:space="preserve">0473</t>
   </si>
   <si>
-    <t xml:space="preserve">9954</t>
+    <t xml:space="preserve">9554</t>
   </si>
   <si>
     <t xml:space="preserve">Bodega Ridge Park</t>
@@ -238,7 +238,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O8" activeCellId="0" sqref="O8"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>